<commit_message>
Cell annotations from Tsang study
</commit_message>
<xml_diff>
--- a/Study-2-Tsang-2014/Annotation_of_Cell_Subpopulations.xlsx
+++ b/Study-2-Tsang-2014/Annotation_of_Cell_Subpopulations.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10507"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dtudk-my.sharepoint.com/personal/s193518_dtu_dk/Documents/Teknisk_Biomedicin/6_semester/Bachelorproject/Study_2-Tsang/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dtudk-my.sharepoint.com/personal/s193518_dtu_dk/Documents/Teknisk_Biomedicin/6_semester/Bachelorproject/Github-Comparative-analysis-CMI-PB/Study-2-Tsang-2014/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="2" documentId="11_8295EE2E33F28FF60F6EBF4F95C0F133E4446FD2" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D9214639-3D37-CA4F-B70D-631CB5CA53F3}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="28800" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="26600" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -3016,8 +3016,8 @@
   </sheetPr>
   <dimension ref="A1:I132"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A74" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="H111" sqref="H111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>